<commit_message>
Changed borough names for consistency between datasets
</commit_message>
<xml_diff>
--- a/data/data-pollution/Population_exceeding_LAEI2016_1_modified.xlsx
+++ b/data/data-pollution/Population_exceeding_LAEI2016_1_modified.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EED9CCF-22EF-5D4F-8944-333298067955}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14400"/>
   </bookViews>
   <sheets>
     <sheet name="Population_exceeding_NO2" sheetId="6" r:id="rId1"/>
     <sheet name="Population_Weighted_Avg_PM2.5" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
-  <si>
-    <t>Barking &amp; Dagenham</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
   <si>
     <t>Barnet</t>
   </si>
@@ -54,9 +50,6 @@
     <t>Hackney</t>
   </si>
   <si>
-    <t>Hammersmith &amp; Fulham</t>
-  </si>
-  <si>
     <t>Haringey</t>
   </si>
   <si>
@@ -73,9 +66,6 @@
   </si>
   <si>
     <t>Islington</t>
-  </si>
-  <si>
-    <t>Kensington &amp; Chelsea</t>
   </si>
   <si>
     <t>Kingston upon Thames</t>
@@ -153,11 +143,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,6 +169,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -204,10 +199,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -221,9 +217,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -314,23 +312,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -366,23 +347,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -558,116 +522,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3.7953795379537955E-2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.6949152542372881E-2</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
-        <v>3.7953795379537955E-2</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1.6949152542372881E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="B5" s="5">
+        <v>0.11479028697571744</v>
+      </c>
+      <c r="C5" s="5">
+        <v>9.841269841269841E-2</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5">
-        <v>0.11479028697571744</v>
-      </c>
-      <c r="C4" s="5">
-        <v>9.841269841269841E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="5">
+        <v>8.5470085470085479E-3</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3.3444816053511705E-3</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5">
-        <v>8.5470085470085479E-3</v>
-      </c>
-      <c r="C5" s="5">
-        <v>3.3444816053511705E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="B7" s="5">
+        <v>0.21806451612903227</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.21305418719211822</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5">
-        <v>0.21806451612903227</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.21305418719211822</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="B8" s="5">
+        <v>4.0322580645161289E-3</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1.29366106080207E-3</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5">
-        <v>4.0322580645161289E-3</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1.29366106080207E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="5">
+      <c r="B9" s="5">
         <v>0.69282511210762332</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C9" s="5">
         <v>0.80439121756487031</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>7</v>
       </c>
       <c r="B10" s="5">
         <v>3.8501560874089492E-2</v>
@@ -675,10 +661,13 @@
       <c r="C10" s="5">
         <v>4.0404040404040404E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E10" s="9"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5">
         <v>0.15504807692307693</v>
@@ -686,10 +675,13 @@
       <c r="C11" s="5">
         <v>0.12311265969802555</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E11" s="9"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5">
         <v>6.2206572769953054E-2</v>
@@ -697,10 +689,13 @@
       <c r="C12" s="5">
         <v>3.5267349260523322E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E12" s="9"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5">
         <v>0.12143928035982009</v>
@@ -708,10 +703,13 @@
       <c r="C13" s="5">
         <v>7.254623044096728E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E13" s="9"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="5">
         <v>0.44444444444444442</v>
@@ -719,10 +717,13 @@
       <c r="C14" s="5">
         <v>0.52359208523592082</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E14" s="9"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5">
         <v>0.5252808988764045</v>
@@ -730,10 +731,13 @@
       <c r="C15" s="5">
         <v>0.46883468834688347</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E15" s="9"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="5">
         <v>0.18630573248407642</v>
@@ -741,10 +745,13 @@
       <c r="C16" s="5">
         <v>0.14503816793893129</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E16" s="9"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="5">
         <v>6.7340067340067337E-3</v>
@@ -752,10 +759,13 @@
       <c r="C17" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E17" s="9"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="5">
         <v>3.5714285714285713E-3</v>
@@ -763,10 +773,13 @@
       <c r="C18" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E18" s="9"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="5">
         <v>2.2408963585434174E-2</v>
@@ -774,10 +787,13 @@
       <c r="C19" s="5">
         <v>1.3089005235602094E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E19" s="9"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="5">
         <v>0.12283464566929134</v>
@@ -785,10 +801,13 @@
       <c r="C20" s="5">
         <v>8.3707025411061287E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E20" s="9"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="5">
         <v>0.6470588235294118</v>
@@ -796,10 +815,13 @@
       <c r="C21" s="5">
         <v>0.74193548387096775</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E21" s="9"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="B22" s="5">
         <v>0.89419795221843001</v>
@@ -807,10 +829,13 @@
       <c r="C22" s="5">
         <v>0.94719471947194722</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E22" s="9"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B23" s="5">
         <v>5.3333333333333337E-2</v>
@@ -818,10 +843,13 @@
       <c r="C23" s="5">
         <v>1.9950124688279301E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E23" s="9"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B24" s="5">
         <v>0.46153846153846156</v>
@@ -829,10 +857,13 @@
       <c r="C24" s="5">
         <v>0.42406015037593986</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E24" s="9"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B25" s="5">
         <v>0.15804597701149425</v>
@@ -840,10 +871,13 @@
       <c r="C25" s="5">
         <v>0.10694444444444444</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E25" s="9"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B26" s="5">
         <v>5.9071729957805907E-2</v>
@@ -851,10 +885,13 @@
       <c r="C26" s="5">
         <v>1.8218623481781375E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E26" s="9"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B27" s="5">
         <v>0.15481651376146788</v>
@@ -862,10 +899,13 @@
       <c r="C27" s="5">
         <v>0.1277533039647577</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E27" s="9"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B28" s="5">
         <v>6.9010416666666671E-2</v>
@@ -873,10 +913,13 @@
       <c r="C28" s="5">
         <v>4.5283018867924525E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E28" s="9"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B29" s="5">
         <v>6.741573033707865E-2</v>
@@ -884,10 +927,13 @@
       <c r="C29" s="5">
         <v>2.7718550106609809E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E29" s="9"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B30" s="5">
         <v>0.54573643410852712</v>
@@ -895,10 +941,13 @@
       <c r="C30" s="5">
         <v>0.58875739644970415</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E30" s="9"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B31" s="5">
         <v>4.2283298097251587E-3</v>
@@ -906,10 +955,13 @@
       <c r="C31" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E31" s="9"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B32" s="5">
         <v>0.58346333853354138</v>
@@ -917,10 +969,13 @@
       <c r="C32" s="5">
         <v>0.77183098591549293</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E32" s="9"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B33" s="5">
         <v>0.11390532544378698</v>
@@ -928,10 +983,13 @@
       <c r="C33" s="5">
         <v>8.5714285714285715E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E33" s="9"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B34" s="5">
         <v>0.30882352941176472</v>
@@ -939,10 +997,13 @@
       <c r="C34" s="5">
         <v>0.23076923076923078</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E34" s="9"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B35" s="5">
         <v>0.87259615384615385</v>
@@ -950,8 +1011,11 @@
       <c r="C35" s="5">
         <v>0.96137339055793991</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E35" s="9"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
     </row>
@@ -965,289 +1029,289 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7">
         <v>12.825305914223813</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="7">
         <v>13.009562455262898</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7">
         <v>12.555151416857141</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="7">
         <v>13.378865101899599</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="7">
         <v>12.406230711484669</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="7">
         <v>14.464092640826106</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8" s="7">
         <v>15.662752559663916</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="7">
         <v>12.717162769431173</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="7">
         <v>13.204130647702454</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="7">
         <v>12.755496880821203</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="7">
         <v>13.176629971988081</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="7">
         <v>13.957765740892315</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" s="7">
         <v>13.928693649285814</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="7">
         <v>13.366428257702827</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="7">
         <v>12.596774197238634</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="7">
         <v>12.055270444076685</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="7">
         <v>12.460866787149298</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" s="7">
         <v>12.916793597145318</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="7">
         <v>14.242613164508223</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B21" s="7">
         <v>14.493944093137564</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" s="7">
         <v>12.7442339846503</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" s="7">
         <v>13.892891901605271</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B24" s="7">
         <v>13.296603213257038</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" s="7">
         <v>13.100079970993649</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B26" s="7">
         <v>13.497564528765302</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B27" s="7">
         <v>12.865967086834058</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B28" s="7">
         <v>12.841997848359711</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B29" s="7">
         <v>14.016861247241872</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B30" s="7">
         <v>12.667020838456564</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B31" s="7">
         <v>14.240919123577294</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B32" s="7">
         <v>13.19053715916146</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B33" s="7">
         <v>13.596722636839669</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B34" s="7">
         <v>15.000195593387213</v>

</xml_diff>